<commit_message>
update before CVS file
</commit_message>
<xml_diff>
--- a/Big O graph.xlsx
+++ b/Big O graph.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="17600" tabRatio="500" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16420" tabRatio="500" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -120,7 +120,6 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
-      <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -336,11 +335,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2052951248"/>
-        <c:axId val="-2056064240"/>
+        <c:axId val="-2087790928"/>
+        <c:axId val="-2059402960"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2052951248"/>
+        <c:axId val="-2087790928"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -397,12 +396,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2056064240"/>
+        <c:crossAx val="-2059402960"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2056064240"/>
+        <c:axId val="-2059402960"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -459,7 +458,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2052951248"/>
+        <c:crossAx val="-2087790928"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -537,11 +536,10 @@
         <a:lstStyle/>
         <a:p>
           <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" cap="none" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="85000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -568,41 +566,55 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n squared</c:v>
+                  <c:v>n</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent1"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent1">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent1"/>
+                <a:schemeClr val="accent1">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent1"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent1">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$5</c:f>
+              <c:f>Sheet2!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -614,27 +626,45 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$B$2:$B$5</c:f>
+              <c:f>Sheet2!$B$2:$B$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.000100970268249512</c:v>
+                  <c:v>0.000157</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000145971</c:v>
+                  <c:v>1.59E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000326991</c:v>
+                  <c:v>3.89E-5</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.00094896</c:v>
+                  <c:v>6.6E-5</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>7.8E-5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.000142</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.000211</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -650,41 +680,55 @@
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>n</c:v>
+                  <c:v>n squared</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
           </c:tx>
           <c:spPr>
-            <a:ln w="19050" cap="rnd">
+            <a:ln w="22225" cap="rnd">
               <a:solidFill>
                 <a:schemeClr val="accent2"/>
               </a:solidFill>
-              <a:round/>
             </a:ln>
-            <a:effectLst/>
+            <a:effectLst>
+              <a:glow rad="139700">
+                <a:schemeClr val="accent2">
+                  <a:satMod val="175000"/>
+                  <a:alpha val="14000"/>
+                </a:schemeClr>
+              </a:glow>
+            </a:effectLst>
           </c:spPr>
           <c:marker>
             <c:symbol val="circle"/>
-            <c:size val="5"/>
+            <c:size val="3"/>
             <c:spPr>
               <a:solidFill>
-                <a:schemeClr val="accent2"/>
+                <a:schemeClr val="accent2">
+                  <a:lumMod val="60000"/>
+                  <a:lumOff val="40000"/>
+                </a:schemeClr>
               </a:solidFill>
-              <a:ln w="9525">
-                <a:solidFill>
-                  <a:schemeClr val="accent2"/>
-                </a:solidFill>
+              <a:ln>
+                <a:noFill/>
               </a:ln>
-              <a:effectLst/>
+              <a:effectLst>
+                <a:glow rad="63500">
+                  <a:schemeClr val="accent2">
+                    <a:satMod val="175000"/>
+                    <a:alpha val="25000"/>
+                  </a:schemeClr>
+                </a:glow>
+              </a:effectLst>
             </c:spPr>
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet2!$A$2:$A$5</c:f>
+              <c:f>Sheet2!$A$2:$A$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>2.0</c:v>
                 </c:pt>
@@ -696,27 +740,45 @@
                 </c:pt>
                 <c:pt idx="3">
                   <c:v>100.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>150.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>300.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1000.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet2!$C$2:$C$5</c:f>
+              <c:f>Sheet2!$C$2:$C$8</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
-                  <c:v>0.000128984451293945</c:v>
+                  <c:v>0.000929</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.000128</c:v>
+                  <c:v>4.39E-5</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.000138044</c:v>
+                  <c:v>0.000383</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.000184953</c:v>
+                  <c:v>0.00118</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.00296</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.01025</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.07</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -731,11 +793,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="-2079661968"/>
-        <c:axId val="-2047511600"/>
+        <c:axId val="-2054682400"/>
+        <c:axId val="-2048712464"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="-2079661968"/>
+        <c:axId val="-2054682400"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -745,9 +807,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -762,12 +825,7 @@
         <c:spPr>
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
-              </a:schemeClr>
-            </a:solidFill>
+            <a:noFill/>
             <a:round/>
           </a:ln>
           <a:effectLst/>
@@ -779,9 +837,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -792,12 +849,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2047511600"/>
+        <c:crossAx val="-2048712464"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2047511600"/>
+        <c:axId val="-2048712464"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -807,9 +864,10 @@
           <c:spPr>
             <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
+                <a:schemeClr val="dk1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                  <a:alpha val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:round/>
@@ -824,9 +882,8 @@
           <a:noFill/>
           <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
             <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="25000"/>
-                <a:lumOff val="75000"/>
+              <a:schemeClr val="lt1">
+                <a:lumMod val="50000"/>
               </a:schemeClr>
             </a:solidFill>
             <a:round/>
@@ -840,9 +897,8 @@
             <a:pPr>
               <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
                 <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
+                  <a:schemeClr val="lt1">
+                    <a:lumMod val="75000"/>
                   </a:schemeClr>
                 </a:solidFill>
                 <a:latin typeface="+mn-lt"/>
@@ -853,7 +909,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2079661968"/>
+        <c:crossAx val="-2054682400"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -866,7 +922,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="t"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -883,9 +939,8 @@
           <a:pPr>
             <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
               <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
+                <a:schemeClr val="lt1">
+                  <a:lumMod val="75000"/>
                 </a:schemeClr>
               </a:solidFill>
               <a:latin typeface="+mn-lt"/>
@@ -903,11 +958,14 @@
   </c:chart>
   <c:spPr>
     <a:solidFill>
-      <a:schemeClr val="bg1"/>
+      <a:schemeClr val="dk1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
     </a:solidFill>
     <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
       <a:solidFill>
-        <a:schemeClr val="tx1">
+        <a:schemeClr val="dk1">
           <a:lumMod val="15000"/>
           <a:lumOff val="85000"/>
         </a:schemeClr>
@@ -1531,211 +1589,35 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="245">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
+    <cs:defRPr sz="900" b="1" kern="1200"/>
   </cs:axisTitle>
   <cs:categoryAxis>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
+  <cs:chartArea>
+    <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
       <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
@@ -1746,16 +1628,296 @@
       </a:solidFill>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="15000"/>
+        <a:lumOff val="85000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:miter lim="800000"/>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="22225" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+      <a:effectLst>
+        <a:glow rad="139700">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="14000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:effectRef>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr">
+          <a:lumMod val="60000"/>
+          <a:lumOff val="40000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:effectLst>
+        <a:glow rad="63500">
+          <a:schemeClr val="phClr">
+            <a:satMod val="175000"/>
+            <a:alpha val="25000"/>
+          </a:schemeClr>
+        </a:glow>
+      </a:effectLst>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="3"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="50000"/>
+          <a:lumOff val="50000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
+            <a:alpha val="75000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
@@ -1765,80 +1927,10 @@
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+          <a:schemeClr val="dk1">
             <a:lumMod val="65000"/>
             <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
+            <a:alpha val="25000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1850,14 +1942,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
             <a:lumMod val="50000"/>
-            <a:lumOff val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1869,14 +1960,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1888,27 +1978,26 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
   </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+  <cs:plotArea3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
   </cs:plotArea3D>
   <cs:seriesAxis>
@@ -1916,9 +2005,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1928,14 +2016,13 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -1947,12 +2034,11 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="85000"/>
       </a:schemeClr>
     </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+    <cs:defRPr sz="1400" b="1" kern="1200" cap="none" baseline="0"/>
   </cs:title>
   <cs:trendline>
     <cs:lnRef idx="0">
@@ -1961,14 +2047,15 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
+      <a:schemeClr val="lt1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="25400" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr">
+            <a:alpha val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
       </a:ln>
     </cs:spPr>
   </cs:trendline>
@@ -1977,9 +2064,8 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:defRPr sz="900" kern="1200"/>
@@ -1989,17 +2075,18 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
+      <a:schemeClr val="dk1"/>
     </cs:fontRef>
     <cs:spPr>
       <a:solidFill>
-        <a:schemeClr val="lt1"/>
+        <a:schemeClr val="lt1">
+          <a:lumMod val="85000"/>
+        </a:schemeClr>
       </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
@@ -2011,37 +2098,30 @@
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
+      <a:schemeClr val="lt1">
+        <a:lumMod val="75000"/>
       </a:schemeClr>
     </cs:fontRef>
     <cs:spPr>
       <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
         <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
+          <a:schemeClr val="lt1">
+            <a:lumMod val="50000"/>
           </a:schemeClr>
         </a:solidFill>
         <a:round/>
       </a:ln>
     </cs:spPr>
     <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr/>
   </cs:valueAxis>
   <cs:wall>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
     <cs:effectRef idx="0"/>
     <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
   </cs:wall>
 </cs:chartStyle>
 </file>
@@ -2595,15 +2675,16 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:C5"/>
+  <dimension ref="A1:C8"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:C5"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="11.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
@@ -2611,10 +2692,10 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
+        <v>4</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
-      </c>
-      <c r="C1" t="s">
-        <v>4</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -2622,10 +2703,10 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>1.00970268249512E-4</v>
+        <v>1.5699999999999999E-4</v>
       </c>
       <c r="C2">
-        <v>1.2898445129394499E-4</v>
+        <v>9.2900000000000003E-4</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -2633,10 +2714,10 @@
         <v>10</v>
       </c>
       <c r="B3">
-        <v>1.45971E-4</v>
+        <v>1.59E-5</v>
       </c>
       <c r="C3">
-        <v>1.2799999999999999E-4</v>
+        <v>4.3900000000000003E-5</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -2644,10 +2725,10 @@
         <v>50</v>
       </c>
       <c r="B4">
-        <v>3.26991E-4</v>
+        <v>3.8899999999999997E-5</v>
       </c>
       <c r="C4">
-        <v>1.3804400000000001E-4</v>
+        <v>3.8299999999999999E-4</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
@@ -2655,10 +2736,43 @@
         <v>100</v>
       </c>
       <c r="B5">
-        <v>9.4895999999999999E-4</v>
+        <v>6.6000000000000005E-5</v>
       </c>
       <c r="C5">
-        <v>1.8495299999999999E-4</v>
+        <v>1.1800000000000001E-3</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6">
+        <v>150</v>
+      </c>
+      <c r="B6">
+        <v>7.7999999999999999E-5</v>
+      </c>
+      <c r="C6">
+        <v>2.96E-3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7">
+        <v>300</v>
+      </c>
+      <c r="B7">
+        <v>1.4200000000000001E-4</v>
+      </c>
+      <c r="C7">
+        <v>1.025E-2</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8">
+        <v>1000</v>
+      </c>
+      <c r="B8">
+        <v>2.1100000000000001E-4</v>
+      </c>
+      <c r="C8">
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
   </sheetData>

</xml_diff>